<commit_message>
docs: edit fields for actions history
</commit_message>
<xml_diff>
--- a/docs/actions_history.xlsx
+++ b/docs/actions_history.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>Model</t>
   </si>
@@ -118,9 +118,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -218,6 +215,15 @@
   </si>
   <si>
     <t>PROGRESSION_REMOVE</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>participation</t>
+  </si>
+  <si>
+    <t>route</t>
   </si>
 </sst>
 </file>
@@ -241,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +257,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -279,13 +291,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,7 +738,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,149 +752,149 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -883,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,220 +928,229 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1148,89 +1178,89 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>